<commit_message>
Editado o método transformEntityIntoRow() para que imprima conteudo dinamico porém ainda não consegue imprimir todo o conteudo adequadamente (falta fazer com que imprima todos os componentes da Row e de todas as planilhas, Creio que a solução passa por fazer iterações genericas nos indices do array $data); Adicionado dois métodos ao SearchComponent.php 1º (listAllOffersByUser) lista todas as ofertas por user_id e o 2º (listAllProductsByStore) que lista todos os produtos por store_id.
</commit_message>
<xml_diff>
--- a/tmp/spreadsheet/Username-Planilha-Produtos.xlsx
+++ b/tmp/spreadsheet/Username-Planilha-Produtos.xlsx
@@ -16,30 +16,33 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="8">
-  <si>
-    <t>Produto</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="9">
+  <si>
+    <t>Nome do Produto</t>
   </si>
   <si>
     <t>Quantidade</t>
   </si>
   <si>
+    <t>Vendidos</t>
+  </si>
+  <si>
     <t>Preço</t>
   </si>
   <si>
-    <t>Produto 1</t>
-  </si>
-  <si>
-    <t>Oferta</t>
-  </si>
-  <si>
-    <t>Descrição</t>
-  </si>
-  <si>
-    <t>Data de Inicio</t>
-  </si>
-  <si>
-    <t>Data de Fim</t>
+    <t>Bacon T</t>
+  </si>
+  <si>
+    <t>Cama X</t>
+  </si>
+  <si>
+    <t>Nome da Oferta</t>
+  </si>
+  <si>
+    <t>Data Inicio</t>
+  </si>
+  <si>
+    <t>Data Fim</t>
   </si>
 </sst>
 </file>
@@ -62,7 +65,7 @@
       <i val="0"/>
       <strike val="0"/>
       <u val="none"/>
-      <sz val="15"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
@@ -79,7 +82,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF1D9D74"/>
+        <fgColor rgb="FF333333"/>
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
@@ -396,10 +399,10 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -407,9 +410,10 @@
     <col min="1" max="1" width="30" customWidth="true" style="0"/>
     <col min="2" max="2" width="30" customWidth="true" style="0"/>
     <col min="3" max="3" width="30" customWidth="true" style="0"/>
+    <col min="4" max="4" width="30" customWidth="true" style="0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -419,16 +423,18 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
         <v>5</v>
-      </c>
-      <c r="C2">
-        <v>5.46</v>
       </c>
     </row>
   </sheetData>
@@ -452,27 +458,32 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="0" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col min="1" max="1" width="30" customWidth="true" style="0"/>
+    <col min="2" max="2" width="30" customWidth="true" style="0"/>
+    <col min="3" max="3" width="30" customWidth="true" style="0"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" t="s">
+    <row r="1" spans="1:3">
+      <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D1" t="s">
+      <c r="B1" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="C1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2"/>
     </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>

</xml_diff>

<commit_message>
Editado os métodos "listAllOffersByUser" e "listAllProductsByStore" do arquivo SearchComponent.php para receber como parametro um array contendo os campos do select; Editado o método "transformEntityIntoRow" para gerar 100% dinamicamente as tabelas, foi adicionado um condicional para checar se a propriedade é um objeto (tem de ser modificado pra primitivo), adicionado um parametro com um array contendo os arrays com os parametros a serem retornados pela consulta ao Banco.
</commit_message>
<xml_diff>
--- a/tmp/spreadsheet/Username-Planilha-Produtos.xlsx
+++ b/tmp/spreadsheet/Username-Planilha-Produtos.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="12">
   <si>
     <t>Nome do Produto</t>
   </si>
@@ -43,6 +43,15 @@
   </si>
   <si>
     <t>Data Fim</t>
+  </si>
+  <si>
+    <t>Oferta 1</t>
+  </si>
+  <si>
+    <t>2015-08-11 00:00:00</t>
+  </si>
+  <si>
+    <t>2019-11-11 00:00:00</t>
   </si>
 </sst>
 </file>
@@ -431,10 +440,28 @@
       <c r="A2" t="s">
         <v>4</v>
       </c>
+      <c r="B2">
+        <v>900</v>
+      </c>
+      <c r="C2">
+        <v>1200</v>
+      </c>
+      <c r="D2">
+        <v>5</v>
+      </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>5</v>
+      </c>
+      <c r="B3">
+        <v>20</v>
+      </c>
+      <c r="C3">
+        <v>40</v>
+      </c>
+      <c r="D3">
+        <v>550.5</v>
       </c>
     </row>
   </sheetData>
@@ -483,7 +510,15 @@
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2"/>
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
     </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>

</xml_diff>